<commit_message>
Updated invoice routing and dynamic Excel file handling
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -437,7 +437,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Z15"/>
+  <dimension ref="A1:Z29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1987,6 +1987,1441 @@
         </is>
       </c>
     </row>
+    <row r="16">
+      <c r="A16" s="3" t="inlineStr">
+        <is>
+          <t>67</t>
+        </is>
+      </c>
+      <c r="B16" s="4" t="n">
+        <v>45404</v>
+      </c>
+      <c r="C16" s="3" t="n">
+        <v>7672</v>
+      </c>
+      <c r="D16" s="3" t="n">
+        <v>14</v>
+      </c>
+      <c r="E16" s="3" t="inlineStr">
+        <is>
+          <t>Other Reimbursement</t>
+        </is>
+      </c>
+      <c r="F16" s="3" t="inlineStr">
+        <is>
+          <t>14/2024-2025/7672</t>
+        </is>
+      </c>
+      <c r="G16" s="3" t="inlineStr">
+        <is>
+          <t>07/04/2024</t>
+        </is>
+      </c>
+      <c r="H16" s="3" t="inlineStr">
+        <is>
+          <t>100009</t>
+        </is>
+      </c>
+      <c r="I16" s="3" t="inlineStr">
+        <is>
+          <t>Nirmal  Kizhakkeveetil</t>
+        </is>
+      </c>
+      <c r="J16" s="3" t="inlineStr">
+        <is>
+          <t>nirmal.k@jfs.in</t>
+        </is>
+      </c>
+      <c r="K16" s="3" t="inlineStr">
+        <is>
+          <t>8104912602</t>
+        </is>
+      </c>
+      <c r="L16" s="3" t="inlineStr"/>
+      <c r="M16" s="3" t="inlineStr"/>
+      <c r="N16" s="3" t="inlineStr">
+        <is>
+          <t>602001532357</t>
+        </is>
+      </c>
+      <c r="O16" s="3" t="inlineStr">
+        <is>
+          <t>ICIC0001417</t>
+        </is>
+      </c>
+      <c r="P16" s="3" t="n">
+        <v>14215.5</v>
+      </c>
+      <c r="Q16" s="3" t="n">
+        <v>14215.5</v>
+      </c>
+      <c r="R16" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="S16" s="3" t="n">
+        <v>14215.5</v>
+      </c>
+      <c r="T16" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="U16" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="V16" s="3" t="n">
+        <v>14215.5</v>
+      </c>
+      <c r="W16" s="3" t="n">
+        <v>14215.5</v>
+      </c>
+      <c r="X16" s="3" t="inlineStr">
+        <is>
+          <t>Trip to Mumbai - Payment SaaS proposal between JFS and JPL approved and responsibilty of the L1 manager Ramesh Radhakrishna</t>
+        </is>
+      </c>
+      <c r="Y16" s="3" t="inlineStr">
+        <is>
+          <t>Exceeded daily limit</t>
+        </is>
+      </c>
+      <c r="Z16" s="3" t="inlineStr">
+        <is>
+          <t>VikasTiwari</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="3" t="inlineStr">
+        <is>
+          <t>67</t>
+        </is>
+      </c>
+      <c r="B17" s="4" t="n">
+        <v>45404</v>
+      </c>
+      <c r="C17" s="3" t="n">
+        <v>7713</v>
+      </c>
+      <c r="D17" s="3" t="n">
+        <v>14</v>
+      </c>
+      <c r="E17" s="3" t="inlineStr">
+        <is>
+          <t>Other Reimbursement</t>
+        </is>
+      </c>
+      <c r="F17" s="3" t="inlineStr">
+        <is>
+          <t>14/2024-2025/7713</t>
+        </is>
+      </c>
+      <c r="G17" s="3" t="inlineStr">
+        <is>
+          <t>08/04/2024</t>
+        </is>
+      </c>
+      <c r="H17" s="3" t="inlineStr">
+        <is>
+          <t>100019</t>
+        </is>
+      </c>
+      <c r="I17" s="3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Shyam Sunder R </t>
+        </is>
+      </c>
+      <c r="J17" s="3" t="inlineStr">
+        <is>
+          <t>shyam.sunder@jfs.in</t>
+        </is>
+      </c>
+      <c r="K17" s="3" t="inlineStr">
+        <is>
+          <t>7021585531</t>
+        </is>
+      </c>
+      <c r="L17" s="3" t="inlineStr"/>
+      <c r="M17" s="3" t="inlineStr"/>
+      <c r="N17" s="3" t="inlineStr">
+        <is>
+          <t>10000004330</t>
+        </is>
+      </c>
+      <c r="O17" s="3" t="inlineStr">
+        <is>
+          <t>IDFB0040101</t>
+        </is>
+      </c>
+      <c r="P17" s="3" t="n">
+        <v>15865</v>
+      </c>
+      <c r="Q17" s="3" t="n">
+        <v>15865</v>
+      </c>
+      <c r="R17" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="S17" s="3" t="n">
+        <v>15865</v>
+      </c>
+      <c r="T17" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="U17" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="V17" s="3" t="n">
+        <v>15865</v>
+      </c>
+      <c r="W17" s="3" t="n">
+        <v>15865</v>
+      </c>
+      <c r="X17" s="3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Date: 13-Mar-2024 Invoice No: TI-0019-8560 DEA MEAL </t>
+        </is>
+      </c>
+      <c r="Y17" s="3" t="inlineStr">
+        <is>
+          <t>Exceeded daily limit</t>
+        </is>
+      </c>
+      <c r="Z17" s="3" t="inlineStr">
+        <is>
+          <t>VikasTiwari</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="3" t="inlineStr">
+        <is>
+          <t>67</t>
+        </is>
+      </c>
+      <c r="B18" s="4" t="n">
+        <v>45404</v>
+      </c>
+      <c r="C18" s="3" t="n">
+        <v>7742</v>
+      </c>
+      <c r="D18" s="3" t="n">
+        <v>13</v>
+      </c>
+      <c r="E18" s="3" t="inlineStr">
+        <is>
+          <t>Local Conveyance and Toll Tax</t>
+        </is>
+      </c>
+      <c r="F18" s="3" t="inlineStr">
+        <is>
+          <t>13/2024-2025/7742</t>
+        </is>
+      </c>
+      <c r="G18" s="3" t="inlineStr">
+        <is>
+          <t>10/04/2024</t>
+        </is>
+      </c>
+      <c r="H18" s="3" t="inlineStr">
+        <is>
+          <t>100008</t>
+        </is>
+      </c>
+      <c r="I18" s="3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">V Mohana  </t>
+        </is>
+      </c>
+      <c r="J18" s="3" t="inlineStr">
+        <is>
+          <t>mohana.v@jfs.in</t>
+        </is>
+      </c>
+      <c r="K18" s="3" t="inlineStr">
+        <is>
+          <t>7977098168</t>
+        </is>
+      </c>
+      <c r="L18" s="3" t="inlineStr"/>
+      <c r="M18" s="3" t="inlineStr"/>
+      <c r="N18" s="3" t="inlineStr">
+        <is>
+          <t>50100098721040</t>
+        </is>
+      </c>
+      <c r="O18" s="3" t="inlineStr">
+        <is>
+          <t>HDFC0000549</t>
+        </is>
+      </c>
+      <c r="P18" s="3" t="n">
+        <v>1553</v>
+      </c>
+      <c r="Q18" s="3" t="n">
+        <v>1552.25</v>
+      </c>
+      <c r="R18" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="S18" s="3" t="n">
+        <v>1552.25</v>
+      </c>
+      <c r="T18" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="U18" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="V18" s="3" t="n">
+        <v>1552.25</v>
+      </c>
+      <c r="W18" s="3" t="n">
+        <v>1552.25</v>
+      </c>
+      <c r="X18" s="3" t="inlineStr">
+        <is>
+          <t>DAKC to Maker - postal ballot discussion</t>
+        </is>
+      </c>
+      <c r="Y18" s="3" t="inlineStr">
+        <is>
+          <t>Exceeded daily limit</t>
+        </is>
+      </c>
+      <c r="Z18" s="3" t="inlineStr">
+        <is>
+          <t>VikasTiwari</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="3" t="inlineStr">
+        <is>
+          <t>74</t>
+        </is>
+      </c>
+      <c r="B19" s="4" t="n">
+        <v>45420</v>
+      </c>
+      <c r="C19" s="3" t="n">
+        <v>7880</v>
+      </c>
+      <c r="D19" s="3" t="n">
+        <v>17</v>
+      </c>
+      <c r="E19" s="3" t="inlineStr">
+        <is>
+          <t>Handset Reimbursement</t>
+        </is>
+      </c>
+      <c r="F19" s="3" t="inlineStr">
+        <is>
+          <t>17/2024-2025/7880</t>
+        </is>
+      </c>
+      <c r="G19" s="3" t="inlineStr">
+        <is>
+          <t>18/04/2024</t>
+        </is>
+      </c>
+      <c r="H19" s="3" t="inlineStr">
+        <is>
+          <t>100013</t>
+        </is>
+      </c>
+      <c r="I19" s="3" t="inlineStr">
+        <is>
+          <t>Sanjay  Rastogi</t>
+        </is>
+      </c>
+      <c r="J19" s="3" t="inlineStr">
+        <is>
+          <t>sanjay.rastogi@jfs.in</t>
+        </is>
+      </c>
+      <c r="K19" s="3" t="inlineStr">
+        <is>
+          <t>0000000016</t>
+        </is>
+      </c>
+      <c r="L19" s="3" t="inlineStr"/>
+      <c r="M19" s="3" t="inlineStr"/>
+      <c r="N19" s="3" t="inlineStr">
+        <is>
+          <t>Cheque</t>
+        </is>
+      </c>
+      <c r="O19" s="3" t="inlineStr">
+        <is>
+          <t>HDFC0000831</t>
+        </is>
+      </c>
+      <c r="P19" s="3" t="n">
+        <v>20000</v>
+      </c>
+      <c r="Q19" s="3" t="n">
+        <v>20000</v>
+      </c>
+      <c r="R19" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="S19" s="3" t="n">
+        <v>20000</v>
+      </c>
+      <c r="T19" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="U19" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="V19" s="3" t="n">
+        <v>20000</v>
+      </c>
+      <c r="W19" s="3" t="n">
+        <v>20000</v>
+      </c>
+      <c r="X19" s="3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Approved as per policy  (Bill No is FANOOI2500007905) </t>
+        </is>
+      </c>
+      <c r="Y19" s="3" t="inlineStr">
+        <is>
+          <t>Exceeded daily limit</t>
+        </is>
+      </c>
+      <c r="Z19" s="3" t="inlineStr">
+        <is>
+          <t>VikasTiwari</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="3" t="inlineStr">
+        <is>
+          <t>74</t>
+        </is>
+      </c>
+      <c r="B20" s="4" t="n">
+        <v>45420</v>
+      </c>
+      <c r="C20" s="3" t="n">
+        <v>8312</v>
+      </c>
+      <c r="D20" s="3" t="n">
+        <v>13</v>
+      </c>
+      <c r="E20" s="3" t="inlineStr">
+        <is>
+          <t>Local Conveyance and Toll Tax</t>
+        </is>
+      </c>
+      <c r="F20" s="3" t="inlineStr">
+        <is>
+          <t>13/2024-2025/8312</t>
+        </is>
+      </c>
+      <c r="G20" s="3" t="inlineStr">
+        <is>
+          <t>25/04/2024</t>
+        </is>
+      </c>
+      <c r="H20" s="3" t="inlineStr">
+        <is>
+          <t>100005</t>
+        </is>
+      </c>
+      <c r="I20" s="3" t="inlineStr">
+        <is>
+          <t>Nikkesh  Galaa</t>
+        </is>
+      </c>
+      <c r="J20" s="3" t="inlineStr">
+        <is>
+          <t>nikesh.gala@jfs.in</t>
+        </is>
+      </c>
+      <c r="K20" s="3" t="inlineStr">
+        <is>
+          <t>8828406219</t>
+        </is>
+      </c>
+      <c r="L20" s="3" t="inlineStr"/>
+      <c r="M20" s="3" t="inlineStr"/>
+      <c r="N20" s="3" t="inlineStr">
+        <is>
+          <t>50100108331590</t>
+        </is>
+      </c>
+      <c r="O20" s="3" t="inlineStr">
+        <is>
+          <t>HDFC0000831</t>
+        </is>
+      </c>
+      <c r="P20" s="3" t="n">
+        <v>3510</v>
+      </c>
+      <c r="Q20" s="3" t="n">
+        <v>3510</v>
+      </c>
+      <c r="R20" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="S20" s="3" t="n">
+        <v>3510</v>
+      </c>
+      <c r="T20" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="U20" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="V20" s="3" t="n">
+        <v>3510</v>
+      </c>
+      <c r="W20" s="3" t="n">
+        <v>3510</v>
+      </c>
+      <c r="X20" s="3" t="inlineStr">
+        <is>
+          <t>Approved as per HR Policy</t>
+        </is>
+      </c>
+      <c r="Y20" s="3" t="inlineStr">
+        <is>
+          <t>Exceeded daily limit</t>
+        </is>
+      </c>
+      <c r="Z20" s="3" t="inlineStr">
+        <is>
+          <t>VikasTiwari</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="3" t="inlineStr">
+        <is>
+          <t>85</t>
+        </is>
+      </c>
+      <c r="B21" s="4" t="n">
+        <v>45449</v>
+      </c>
+      <c r="C21" s="3" t="n">
+        <v>8466</v>
+      </c>
+      <c r="D21" s="3" t="n">
+        <v>15</v>
+      </c>
+      <c r="E21" s="3" t="inlineStr">
+        <is>
+          <t>Pre Employment Medical</t>
+        </is>
+      </c>
+      <c r="F21" s="3" t="inlineStr">
+        <is>
+          <t>15/2024-2025/8466</t>
+        </is>
+      </c>
+      <c r="G21" s="3" t="inlineStr">
+        <is>
+          <t>10/05/2024</t>
+        </is>
+      </c>
+      <c r="H21" s="3" t="inlineStr">
+        <is>
+          <t>100002</t>
+        </is>
+      </c>
+      <c r="I21" s="3" t="inlineStr">
+        <is>
+          <t>Ketan Y Patil</t>
+        </is>
+      </c>
+      <c r="J21" s="3" t="inlineStr">
+        <is>
+          <t>ketan.patil@jfs.in</t>
+        </is>
+      </c>
+      <c r="K21" s="3" t="inlineStr">
+        <is>
+          <t>9867614335</t>
+        </is>
+      </c>
+      <c r="L21" s="3" t="inlineStr"/>
+      <c r="M21" s="3" t="inlineStr"/>
+      <c r="N21" s="3" t="inlineStr">
+        <is>
+          <t>31431894509</t>
+        </is>
+      </c>
+      <c r="O21" s="3" t="inlineStr">
+        <is>
+          <t>SBIN0013033</t>
+        </is>
+      </c>
+      <c r="P21" s="3" t="n">
+        <v>13000</v>
+      </c>
+      <c r="Q21" s="3" t="n">
+        <v>13000</v>
+      </c>
+      <c r="R21" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="S21" s="3" t="n">
+        <v>13000</v>
+      </c>
+      <c r="T21" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="U21" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="V21" s="3" t="n">
+        <v>13000</v>
+      </c>
+      <c r="W21" s="3" t="n">
+        <v>13000</v>
+      </c>
+      <c r="X21" s="3" t="inlineStr">
+        <is>
+          <t>Periodic medical examination for myself</t>
+        </is>
+      </c>
+      <c r="Y21" s="3" t="inlineStr">
+        <is>
+          <t>Exceeded daily limit</t>
+        </is>
+      </c>
+      <c r="Z21" s="3" t="inlineStr">
+        <is>
+          <t>VikasTiwari</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="3" t="inlineStr">
+        <is>
+          <t>85</t>
+        </is>
+      </c>
+      <c r="B22" s="4" t="n">
+        <v>45449</v>
+      </c>
+      <c r="C22" s="3" t="n">
+        <v>8695</v>
+      </c>
+      <c r="D22" s="3" t="n">
+        <v>13</v>
+      </c>
+      <c r="E22" s="3" t="inlineStr">
+        <is>
+          <t>Local Conveyance and Toll Tax</t>
+        </is>
+      </c>
+      <c r="F22" s="3" t="inlineStr">
+        <is>
+          <t>13/2024-2025/8695</t>
+        </is>
+      </c>
+      <c r="G22" s="3" t="inlineStr">
+        <is>
+          <t>17/05/2024</t>
+        </is>
+      </c>
+      <c r="H22" s="3" t="inlineStr">
+        <is>
+          <t>100045</t>
+        </is>
+      </c>
+      <c r="I22" s="3" t="inlineStr">
+        <is>
+          <t>Tamalika  De</t>
+        </is>
+      </c>
+      <c r="J22" s="3" t="inlineStr">
+        <is>
+          <t>tamalika.de@jfs.in</t>
+        </is>
+      </c>
+      <c r="K22" s="3" t="inlineStr">
+        <is>
+          <t>8451006413</t>
+        </is>
+      </c>
+      <c r="L22" s="3" t="inlineStr"/>
+      <c r="M22" s="3" t="inlineStr"/>
+      <c r="N22" s="3" t="inlineStr">
+        <is>
+          <t>641201500043</t>
+        </is>
+      </c>
+      <c r="O22" s="3" t="inlineStr">
+        <is>
+          <t>ICIC0006412</t>
+        </is>
+      </c>
+      <c r="P22" s="3" t="n">
+        <v>4232.61</v>
+      </c>
+      <c r="Q22" s="3" t="n">
+        <v>4232.61</v>
+      </c>
+      <c r="R22" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="S22" s="3" t="n">
+        <v>4232.61</v>
+      </c>
+      <c r="T22" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="U22" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="V22" s="3" t="n">
+        <v>4232.61</v>
+      </c>
+      <c r="W22" s="3" t="n">
+        <v>4232.61</v>
+      </c>
+      <c r="X22" s="3" t="inlineStr">
+        <is>
+          <t>Vashi to Makers</t>
+        </is>
+      </c>
+      <c r="Y22" s="3" t="inlineStr">
+        <is>
+          <t>Exceeded daily limit</t>
+        </is>
+      </c>
+      <c r="Z22" s="3" t="inlineStr">
+        <is>
+          <t>VikasTiwari</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="3" t="inlineStr">
+        <is>
+          <t>117</t>
+        </is>
+      </c>
+      <c r="B23" s="4" t="n">
+        <v>45523</v>
+      </c>
+      <c r="C23" s="3" t="n">
+        <v>10624</v>
+      </c>
+      <c r="D23" s="3" t="n">
+        <v>14</v>
+      </c>
+      <c r="E23" s="3" t="inlineStr">
+        <is>
+          <t>Other Reimbursement</t>
+        </is>
+      </c>
+      <c r="F23" s="3" t="inlineStr">
+        <is>
+          <t>14/2024-2025/10624</t>
+        </is>
+      </c>
+      <c r="G23" s="3" t="inlineStr">
+        <is>
+          <t>17/07/2024</t>
+        </is>
+      </c>
+      <c r="H23" s="3" t="inlineStr">
+        <is>
+          <t>100071</t>
+        </is>
+      </c>
+      <c r="I23" s="3" t="inlineStr">
+        <is>
+          <t>Prakriti  Jain</t>
+        </is>
+      </c>
+      <c r="J23" s="3" t="inlineStr">
+        <is>
+          <t>prakriti.jain@jfs.in</t>
+        </is>
+      </c>
+      <c r="K23" s="3" t="inlineStr">
+        <is>
+          <t>7568888066</t>
+        </is>
+      </c>
+      <c r="L23" s="3" t="inlineStr"/>
+      <c r="M23" s="3" t="inlineStr"/>
+      <c r="N23" s="3" t="inlineStr">
+        <is>
+          <t>61201136961</t>
+        </is>
+      </c>
+      <c r="O23" s="3" t="inlineStr">
+        <is>
+          <t>SBIN0032082</t>
+        </is>
+      </c>
+      <c r="P23" s="3" t="n">
+        <v>1699</v>
+      </c>
+      <c r="Q23" s="3" t="n">
+        <v>1699</v>
+      </c>
+      <c r="R23" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="S23" s="3" t="n">
+        <v>1699</v>
+      </c>
+      <c r="T23" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="U23" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="V23" s="3" t="n">
+        <v>1699</v>
+      </c>
+      <c r="W23" s="3" t="n">
+        <v>1699</v>
+      </c>
+      <c r="X23" s="3" t="inlineStr">
+        <is>
+          <t>Purchased Rubber stamps for the Company</t>
+        </is>
+      </c>
+      <c r="Y23" s="3" t="inlineStr">
+        <is>
+          <t>Exceeded daily limit</t>
+        </is>
+      </c>
+      <c r="Z23" s="3" t="inlineStr">
+        <is>
+          <t>VikasTiwari</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="3" t="inlineStr">
+        <is>
+          <t>117</t>
+        </is>
+      </c>
+      <c r="B24" s="4" t="n">
+        <v>45523</v>
+      </c>
+      <c r="C24" s="3" t="n">
+        <v>11319</v>
+      </c>
+      <c r="D24" s="3" t="n">
+        <v>16</v>
+      </c>
+      <c r="E24" s="3" t="inlineStr">
+        <is>
+          <t>Travel Accommodation Expenses</t>
+        </is>
+      </c>
+      <c r="F24" s="3" t="inlineStr">
+        <is>
+          <t>16/2024-2025/11319</t>
+        </is>
+      </c>
+      <c r="G24" s="3" t="inlineStr">
+        <is>
+          <t>04/08/2024</t>
+        </is>
+      </c>
+      <c r="H24" s="3" t="inlineStr">
+        <is>
+          <t>100008</t>
+        </is>
+      </c>
+      <c r="I24" s="3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">V Mohana  </t>
+        </is>
+      </c>
+      <c r="J24" s="3" t="inlineStr">
+        <is>
+          <t>mohana.v@jfs.in</t>
+        </is>
+      </c>
+      <c r="K24" s="3" t="inlineStr">
+        <is>
+          <t>7977098168</t>
+        </is>
+      </c>
+      <c r="L24" s="3" t="inlineStr"/>
+      <c r="M24" s="3" t="inlineStr"/>
+      <c r="N24" s="3" t="inlineStr">
+        <is>
+          <t>50100098721040</t>
+        </is>
+      </c>
+      <c r="O24" s="3" t="inlineStr">
+        <is>
+          <t>HDFC0000549</t>
+        </is>
+      </c>
+      <c r="P24" s="3" t="n">
+        <v>10620</v>
+      </c>
+      <c r="Q24" s="3" t="n">
+        <v>10620</v>
+      </c>
+      <c r="R24" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="S24" s="3" t="n">
+        <v>10620</v>
+      </c>
+      <c r="T24" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="U24" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="V24" s="3" t="n">
+        <v>10620</v>
+      </c>
+      <c r="W24" s="3" t="n">
+        <v>10620</v>
+      </c>
+      <c r="X24" s="3" t="inlineStr">
+        <is>
+          <t>went for discussion with DEA officials in connection with FDI approval1</t>
+        </is>
+      </c>
+      <c r="Y24" s="3" t="inlineStr">
+        <is>
+          <t>Exceeded daily limit</t>
+        </is>
+      </c>
+      <c r="Z24" s="3" t="inlineStr">
+        <is>
+          <t>VikasTiwari</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="3" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="B25" s="4" t="n">
+        <v>45482</v>
+      </c>
+      <c r="C25" s="3" t="n">
+        <v>9431</v>
+      </c>
+      <c r="D25" s="3" t="n">
+        <v>13</v>
+      </c>
+      <c r="E25" s="3" t="inlineStr">
+        <is>
+          <t>Local Conveyance and Toll Tax</t>
+        </is>
+      </c>
+      <c r="F25" s="3" t="inlineStr">
+        <is>
+          <t>13/2024-2025/9431</t>
+        </is>
+      </c>
+      <c r="G25" s="3" t="inlineStr">
+        <is>
+          <t>17/06/2024</t>
+        </is>
+      </c>
+      <c r="H25" s="3" t="inlineStr">
+        <is>
+          <t>100019</t>
+        </is>
+      </c>
+      <c r="I25" s="3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Shyam Sunder R </t>
+        </is>
+      </c>
+      <c r="J25" s="3" t="inlineStr">
+        <is>
+          <t>shyam.sunder@jfs.in</t>
+        </is>
+      </c>
+      <c r="K25" s="3" t="inlineStr">
+        <is>
+          <t>7021585531</t>
+        </is>
+      </c>
+      <c r="L25" s="3" t="inlineStr"/>
+      <c r="M25" s="3" t="inlineStr"/>
+      <c r="N25" s="3" t="inlineStr">
+        <is>
+          <t>10000004330</t>
+        </is>
+      </c>
+      <c r="O25" s="3" t="inlineStr">
+        <is>
+          <t>IDFB0040101</t>
+        </is>
+      </c>
+      <c r="P25" s="3" t="n">
+        <v>20302</v>
+      </c>
+      <c r="Q25" s="3" t="n">
+        <v>20302</v>
+      </c>
+      <c r="R25" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="S25" s="3" t="n">
+        <v>20302</v>
+      </c>
+      <c r="T25" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="U25" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="V25" s="3" t="n">
+        <v>20302</v>
+      </c>
+      <c r="W25" s="3" t="n">
+        <v>20302</v>
+      </c>
+      <c r="X25" s="3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Dated 26 Dec, 2023 e-Receipt - 231226441598 This is the bill of a flights taken in last financial year but as the bill were missing I claimed but was rejected so again depositing the same for kind consideration please  </t>
+        </is>
+      </c>
+      <c r="Y25" s="3" t="inlineStr">
+        <is>
+          <t>Exceeded daily limit</t>
+        </is>
+      </c>
+      <c r="Z25" s="3" t="inlineStr">
+        <is>
+          <t>VikasTiwari</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Batch No</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>ClaimID</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>ClaimTypeID</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>Claim Type</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>Claim Code</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>Applied Date</t>
+        </is>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>Entity</t>
+        </is>
+      </c>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>Employee Code</t>
+        </is>
+      </c>
+      <c r="J26" t="inlineStr">
+        <is>
+          <t>Employee Name</t>
+        </is>
+      </c>
+      <c r="K26" t="inlineStr">
+        <is>
+          <t>Email ID</t>
+        </is>
+      </c>
+      <c r="L26" t="inlineStr">
+        <is>
+          <t>Mobile Number</t>
+        </is>
+      </c>
+      <c r="M26" t="inlineStr">
+        <is>
+          <t>Applied Amount/Units</t>
+        </is>
+      </c>
+      <c r="N26" t="inlineStr">
+        <is>
+          <t>Approved Amount/Units</t>
+        </is>
+      </c>
+      <c r="O26" t="inlineStr">
+        <is>
+          <t>Taxable</t>
+        </is>
+      </c>
+      <c r="P26" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q26" t="inlineStr">
+        <is>
+          <t>TDS Amount</t>
+        </is>
+      </c>
+      <c r="R26" t="inlineStr">
+        <is>
+          <t>Advance Amount</t>
+        </is>
+      </c>
+      <c r="S26" t="inlineStr">
+        <is>
+          <t>Payable Amount</t>
+        </is>
+      </c>
+      <c r="T26" t="inlineStr">
+        <is>
+          <t>Net Payable Amount</t>
+        </is>
+      </c>
+      <c r="U26" t="inlineStr">
+        <is>
+          <t>Net Pay(Round Amt)</t>
+        </is>
+      </c>
+      <c r="V26" t="inlineStr">
+        <is>
+          <t>Remarks</t>
+        </is>
+      </c>
+      <c r="Y26" t="inlineStr">
+        <is>
+          <t>Within limit</t>
+        </is>
+      </c>
+      <c r="Z26" t="inlineStr">
+        <is>
+          <t>VikasTiwari</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="3" t="inlineStr">
+        <is>
+          <t>130</t>
+        </is>
+      </c>
+      <c r="B27" s="4" t="n">
+        <v>45551</v>
+      </c>
+      <c r="C27" s="3" t="n">
+        <v>12636</v>
+      </c>
+      <c r="D27" s="3" t="n">
+        <v>14</v>
+      </c>
+      <c r="E27" s="3" t="inlineStr">
+        <is>
+          <t>Other Reimbursement</t>
+        </is>
+      </c>
+      <c r="F27" s="3" t="inlineStr">
+        <is>
+          <t>14/2024-2025/12636</t>
+        </is>
+      </c>
+      <c r="G27" s="3" t="inlineStr">
+        <is>
+          <t>11/09/2024</t>
+        </is>
+      </c>
+      <c r="H27" s="3" t="inlineStr">
+        <is>
+          <t>JFSL</t>
+        </is>
+      </c>
+      <c r="I27" s="3" t="inlineStr">
+        <is>
+          <t>100018</t>
+        </is>
+      </c>
+      <c r="J27" s="3" t="inlineStr">
+        <is>
+          <t>Anusha  Kanumuru</t>
+        </is>
+      </c>
+      <c r="K27" s="3" t="inlineStr">
+        <is>
+          <t>anusha.kanumuru@jfs.in</t>
+        </is>
+      </c>
+      <c r="L27" s="3" t="inlineStr">
+        <is>
+          <t>9885179585</t>
+        </is>
+      </c>
+      <c r="M27" s="3" t="n">
+        <v>20507</v>
+      </c>
+      <c r="N27" s="3" t="n">
+        <v>20507</v>
+      </c>
+      <c r="O27" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="P27" s="3" t="n">
+        <v>20507</v>
+      </c>
+      <c r="Q27" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="R27" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="S27" s="3" t="n">
+        <v>20507</v>
+      </c>
+      <c r="T27" s="3" t="n">
+        <v>20507</v>
+      </c>
+      <c r="U27" s="3" t="n">
+        <v>20507</v>
+      </c>
+      <c r="V27" s="3" t="inlineStr">
+        <is>
+          <t>Team Dinner- For successful first AGM post listing approved and responsibility of the L1 manager Mohana Maam</t>
+        </is>
+      </c>
+      <c r="W27" s="3" t="inlineStr"/>
+      <c r="X27" s="3" t="inlineStr"/>
+      <c r="Y27" s="3" t="inlineStr">
+        <is>
+          <t>Exceeded daily limit</t>
+        </is>
+      </c>
+      <c r="Z27" s="3" t="inlineStr">
+        <is>
+          <t>VikasTiwari</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="3" t="inlineStr">
+        <is>
+          <t>130</t>
+        </is>
+      </c>
+      <c r="B28" s="4" t="n">
+        <v>45551</v>
+      </c>
+      <c r="C28" s="3" t="n">
+        <v>12548</v>
+      </c>
+      <c r="D28" s="3" t="n">
+        <v>13</v>
+      </c>
+      <c r="E28" s="3" t="inlineStr">
+        <is>
+          <t>Local Conveyance and Toll Tax</t>
+        </is>
+      </c>
+      <c r="F28" s="3" t="inlineStr">
+        <is>
+          <t>13/2024-2025/12548</t>
+        </is>
+      </c>
+      <c r="G28" s="3" t="inlineStr">
+        <is>
+          <t>08/09/2024</t>
+        </is>
+      </c>
+      <c r="H28" s="3" t="inlineStr">
+        <is>
+          <t>JFSL</t>
+        </is>
+      </c>
+      <c r="I28" s="3" t="inlineStr">
+        <is>
+          <t>100097</t>
+        </is>
+      </c>
+      <c r="J28" s="3" t="inlineStr">
+        <is>
+          <t>Ritisha  Singh</t>
+        </is>
+      </c>
+      <c r="K28" s="3" t="inlineStr">
+        <is>
+          <t>ritisha.singh@jfs.in</t>
+        </is>
+      </c>
+      <c r="L28" s="3" t="inlineStr">
+        <is>
+          <t>7976891287</t>
+        </is>
+      </c>
+      <c r="M28" s="3" t="n">
+        <v>2652</v>
+      </c>
+      <c r="N28" s="3" t="n">
+        <v>2652</v>
+      </c>
+      <c r="O28" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="P28" s="3" t="n">
+        <v>2652</v>
+      </c>
+      <c r="Q28" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="R28" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="S28" s="3" t="n">
+        <v>2652</v>
+      </c>
+      <c r="T28" s="3" t="n">
+        <v>2652</v>
+      </c>
+      <c r="U28" s="3" t="n">
+        <v>2652</v>
+      </c>
+      <c r="V28" s="3" t="inlineStr">
+        <is>
+          <t>Cab fare for travelling to and from DAKC (Base location is BKC office)</t>
+        </is>
+      </c>
+      <c r="W28" s="3" t="inlineStr"/>
+      <c r="X28" s="3" t="inlineStr"/>
+      <c r="Y28" s="3" t="inlineStr">
+        <is>
+          <t>Exceeded daily limit</t>
+        </is>
+      </c>
+      <c r="Z28" s="3" t="inlineStr">
+        <is>
+          <t>VikasTiwari</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="3" t="inlineStr">
+        <is>
+          <t>130</t>
+        </is>
+      </c>
+      <c r="B29" s="4" t="n">
+        <v>45551</v>
+      </c>
+      <c r="C29" s="3" t="n">
+        <v>12594</v>
+      </c>
+      <c r="D29" s="3" t="n">
+        <v>15</v>
+      </c>
+      <c r="E29" s="3" t="inlineStr">
+        <is>
+          <t>Pre Employment Medical</t>
+        </is>
+      </c>
+      <c r="F29" s="3" t="inlineStr">
+        <is>
+          <t>15/2024-2025/12594</t>
+        </is>
+      </c>
+      <c r="G29" s="3" t="inlineStr">
+        <is>
+          <t>10/09/2024</t>
+        </is>
+      </c>
+      <c r="H29" s="3" t="inlineStr">
+        <is>
+          <t>JFSL</t>
+        </is>
+      </c>
+      <c r="I29" s="3" t="inlineStr">
+        <is>
+          <t>100154</t>
+        </is>
+      </c>
+      <c r="J29" s="3" t="inlineStr">
+        <is>
+          <t>Varun Kumar Bitla</t>
+        </is>
+      </c>
+      <c r="K29" s="3" t="inlineStr">
+        <is>
+          <t>varunkumar.bitla@jfs.in</t>
+        </is>
+      </c>
+      <c r="L29" s="3" t="inlineStr">
+        <is>
+          <t>7842271210</t>
+        </is>
+      </c>
+      <c r="M29" s="3" t="n">
+        <v>1600</v>
+      </c>
+      <c r="N29" s="3" t="n">
+        <v>1600</v>
+      </c>
+      <c r="O29" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="P29" s="3" t="n">
+        <v>1600</v>
+      </c>
+      <c r="Q29" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="R29" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="S29" s="3" t="n">
+        <v>1600</v>
+      </c>
+      <c r="T29" s="3" t="n">
+        <v>1600</v>
+      </c>
+      <c r="U29" s="3" t="n">
+        <v>1600</v>
+      </c>
+      <c r="V29" s="3" t="inlineStr">
+        <is>
+          <t>Following is the bill for my medical expenses for my pre medical examination. Please provide a refund</t>
+        </is>
+      </c>
+      <c r="W29" s="3" t="inlineStr"/>
+      <c r="X29" s="3" t="inlineStr"/>
+      <c r="Y29" s="3" t="inlineStr">
+        <is>
+          <t>Exceeded daily limit</t>
+        </is>
+      </c>
+      <c r="Z29" s="3" t="inlineStr">
+        <is>
+          <t>VikasTiwari</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>